<commit_message>
Changes to inputs and scripts during debugging and finalising of version 1.3
</commit_message>
<xml_diff>
--- a/tests/test_files/Inputs_Batch.xlsx
+++ b/tests/test_files/Inputs_Batch.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC9636-E706-4482-8015-6C2A8F43EC8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DDE3B2-8A01-43A1-9C77-9E2AFC65554E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="814" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1743,9 +1743,6 @@
     <t>Default folder to store log messages and the excel results, this can be overwritten using the GUI</t>
   </si>
   <si>
-    <t>Include_Convex</t>
-  </si>
-  <si>
     <t>Updated to include ConvexHull calculation</t>
   </si>
   <si>
@@ -1819,6 +1816,9 @@
   </si>
   <si>
     <t>TEST Line NC</t>
+  </si>
+  <si>
+    <t>Include_Loci</t>
   </si>
 </sst>
 </file>
@@ -3478,7 +3478,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>168</v>
@@ -3487,12 +3487,12 @@
         <v>44015</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>168</v>
@@ -3501,7 +3501,7 @@
         <v>44030</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,8 +3677,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3807,13 +3807,13 @@
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="B13" s="34" t="b">
         <v>1</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4059,7 +4059,7 @@
   <sheetData>
     <row r="1" spans="1:28" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="64" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="60"/>
@@ -9190,7 +9190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3D923C-DF32-42AB-9854-C26FD0393729}">
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -9214,7 +9214,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="84" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="60"/>
@@ -9275,39 +9275,39 @@
         <v>191</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C4" s="71"/>
       <c r="D4" s="66" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E4" s="68"/>
       <c r="F4" s="66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G4" s="68"/>
       <c r="H4" s="66" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I4" s="68"/>
       <c r="J4" s="66" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K4" s="68"/>
       <c r="L4" s="66" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M4" s="68"/>
       <c r="N4" s="66" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O4" s="68"/>
       <c r="P4" s="66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q4" s="68"/>
       <c r="R4" s="66" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="S4" s="68"/>
     </row>
@@ -9316,55 +9316,55 @@
         <v>0</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="L5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="N5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="O5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="P5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="Q5" s="31" t="s">
         <v>166</v>
       </c>
       <c r="R5" s="29" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S5" s="31" t="s">
         <v>166</v>
@@ -9372,13 +9372,13 @@
     </row>
     <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
@@ -9399,19 +9399,19 @@
     </row>
     <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>248</v>
-      </c>
       <c r="E7" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
@@ -13607,7 +13607,7 @@
         <v>174</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" s="46" t="s">
         <v>175</v>
@@ -14371,7 +14371,7 @@
         <v>187</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="46" t="s">
         <v>189</v>
@@ -14547,26 +14547,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -14718,31 +14698,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14758,4 +14734,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>